<commit_message>
plant local analysis result.
</commit_message>
<xml_diff>
--- a/src/Input/plant.xlsx
+++ b/src/Input/plant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\2023HiMCM\src\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA17EFF-0C60-4611-BA94-B57C76DD9A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE349B2-D102-4304-A6F7-56A5F7D6EC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Plants" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5060" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5173" uniqueCount="887">
   <si>
     <t>scientificName</t>
   </si>
@@ -2689,10 +2689,6 @@
     <t>Impact factor</t>
   </si>
   <si>
-    <t>Location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>State</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2716,6 +2712,46 @@
   </si>
   <si>
     <t>Fine, Medium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coarse, Fine, Medium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coarse, Medium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15-26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-23</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2860,7 +2896,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2901,6 +2937,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3272,9 +3309,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W227"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A227" sqref="A227:XFD227"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -19440,7 +19477,7 @@
   <pageSetup orientation="portrait" r:id="rId7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="14">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="14">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{42764FDD-458C-4BC7-BEC5-7A129C4BD67A}">
           <x14:formula1>
             <xm:f>Help!$A$2:$A$4</xm:f>
@@ -19533,10 +19570,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB99CE73-EB40-4BA3-BA00-617790B0D471}">
-  <dimension ref="A1:AE16"/>
+  <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:Z1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD28" sqref="AD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -19568,11 +19606,12 @@
     <col min="25" max="25" width="14.375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17.875" bestFit="1" customWidth="1"/>
     <col min="27" max="29" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.625" customWidth="1"/>
-    <col min="31" max="31" width="9.375" customWidth="1"/>
+    <col min="30" max="30" width="9.375" customWidth="1"/>
+    <col min="31" max="31" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="14.25">
+    <row r="1" spans="1:32" ht="14.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -19652,22 +19691,25 @@
         <v>699</v>
       </c>
       <c r="AA1" s="15" t="s">
+        <v>873</v>
+      </c>
+      <c r="AB1" s="15" t="s">
         <v>874</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>875</v>
-      </c>
-      <c r="AC1" s="15" t="s">
-        <v>876</v>
       </c>
       <c r="AD1" s="14" t="s">
         <v>870</v>
       </c>
       <c r="AE1" s="14" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31">
+        <v>884</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
       <c r="A2" s="1" t="s">
         <v>413</v>
       </c>
@@ -19734,7 +19776,18 @@
       <c r="V2">
         <v>1</v>
       </c>
-      <c r="W2" s="1"/>
+      <c r="W2" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="X2" t="s">
+        <v>822</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>823</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>822</v>
+      </c>
       <c r="AA2">
         <v>-39</v>
       </c>
@@ -19742,10 +19795,19 @@
         <v>852</v>
       </c>
       <c r="AC2" t="s">
+        <v>876</v>
+      </c>
+      <c r="AD2" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="3" spans="1:31">
+      <c r="AE2" s="16">
+        <v>-34</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>77.105587104977502</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32">
       <c r="A3" s="1" t="s">
         <v>413</v>
       </c>
@@ -19812,7 +19874,18 @@
       <c r="V3">
         <v>1</v>
       </c>
-      <c r="W3" s="1"/>
+      <c r="W3" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="X3" t="s">
+        <v>823</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>824</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>824</v>
+      </c>
       <c r="AA3">
         <v>-39</v>
       </c>
@@ -19820,10 +19893,19 @@
         <v>852</v>
       </c>
       <c r="AC3" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31">
+        <v>876</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>878</v>
+      </c>
+      <c r="AE3" s="16" t="s">
+        <v>885</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>80.246105406143798</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32">
       <c r="A4" s="1" t="s">
         <v>413</v>
       </c>
@@ -19890,7 +19972,18 @@
       <c r="V4">
         <v>1</v>
       </c>
-      <c r="W4" s="1"/>
+      <c r="W4" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="X4" t="s">
+        <v>824</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>822</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>822</v>
+      </c>
       <c r="AA4">
         <v>-39</v>
       </c>
@@ -19898,10 +19991,19 @@
         <v>852</v>
       </c>
       <c r="AC4" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31">
+        <v>876</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>879</v>
+      </c>
+      <c r="AE4" s="16" t="s">
+        <v>886</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>77.105587104977502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -19968,9 +20070,38 @@
       <c r="V5">
         <v>1</v>
       </c>
-      <c r="W5" s="1"/>
-    </row>
-    <row r="6" spans="1:31">
+      <c r="W5" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="X5" t="s">
+        <v>822</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>823</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>822</v>
+      </c>
+      <c r="AA5">
+        <v>-27</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>881</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>880</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>877</v>
+      </c>
+      <c r="AE5" s="16">
+        <v>-34</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>72.316669714999307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
@@ -20037,9 +20168,38 @@
       <c r="V6">
         <v>1</v>
       </c>
-      <c r="W6" s="1"/>
-    </row>
-    <row r="7" spans="1:31">
+      <c r="W6" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="X6" t="s">
+        <v>823</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>824</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>824</v>
+      </c>
+      <c r="AA6">
+        <v>-27</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>881</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>880</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>878</v>
+      </c>
+      <c r="AE6" s="16" t="s">
+        <v>885</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>80.687109031491502</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -20106,9 +20266,38 @@
       <c r="V7">
         <v>1</v>
       </c>
-      <c r="W7" s="1"/>
-    </row>
-    <row r="8" spans="1:31">
+      <c r="W7" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="X7" t="s">
+        <v>824</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>822</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>822</v>
+      </c>
+      <c r="AA7">
+        <v>-27</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>881</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>880</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>879</v>
+      </c>
+      <c r="AE7" s="16" t="s">
+        <v>886</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>74.931630222662307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32">
       <c r="A8" s="1" t="s">
         <v>629</v>
       </c>
@@ -20175,9 +20364,38 @@
       <c r="V8">
         <v>0</v>
       </c>
-      <c r="W8" s="1"/>
-    </row>
-    <row r="9" spans="1:31">
+      <c r="W8" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="X8" t="s">
+        <v>822</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>823</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>822</v>
+      </c>
+      <c r="AA8">
+        <v>-33</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>852</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>880</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>877</v>
+      </c>
+      <c r="AE8" s="16">
+        <v>-34</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>64.627601085086994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32">
       <c r="A9" s="1" t="s">
         <v>629</v>
       </c>
@@ -20244,9 +20462,38 @@
       <c r="V9">
         <v>0</v>
       </c>
-      <c r="W9" s="1"/>
-    </row>
-    <row r="10" spans="1:31">
+      <c r="W9" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="X9" t="s">
+        <v>824</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>824</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>824</v>
+      </c>
+      <c r="AA9">
+        <v>-33</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>852</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>880</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>878</v>
+      </c>
+      <c r="AE9" s="16" t="s">
+        <v>885</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>70.383079893916204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32">
       <c r="A10" s="1" t="s">
         <v>629</v>
       </c>
@@ -20313,9 +20560,38 @@
       <c r="V10">
         <v>0</v>
       </c>
-      <c r="W10" s="1"/>
-    </row>
-    <row r="11" spans="1:31">
+      <c r="W10" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="X10" t="s">
+        <v>823</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>822</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>822</v>
+      </c>
+      <c r="AA10">
+        <v>-33</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>852</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>880</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>879</v>
+      </c>
+      <c r="AE10" s="16" t="s">
+        <v>886</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>64.627601085086994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32">
       <c r="A11" s="1" t="s">
         <v>680</v>
       </c>
@@ -20382,9 +20658,38 @@
       <c r="V11">
         <v>1</v>
       </c>
-      <c r="W11" s="1"/>
-    </row>
-    <row r="12" spans="1:31">
+      <c r="W11" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="X11" t="s">
+        <v>822</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>823</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>822</v>
+      </c>
+      <c r="AA11">
+        <v>-39</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>881</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>880</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>877</v>
+      </c>
+      <c r="AE11" s="16">
+        <v>-34</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>62.295397366888501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32">
       <c r="A12" s="1" t="s">
         <v>680</v>
       </c>
@@ -20451,9 +20756,38 @@
       <c r="V12">
         <v>1</v>
       </c>
-      <c r="W12" s="1"/>
-    </row>
-    <row r="13" spans="1:31">
+      <c r="W12" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="X12" t="s">
+        <v>823</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>824</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>824</v>
+      </c>
+      <c r="AA12">
+        <v>-39</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>881</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>880</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>878</v>
+      </c>
+      <c r="AE12" s="16" t="s">
+        <v>885</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>65.435915668054704</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32">
       <c r="A13" s="1" t="s">
         <v>680</v>
       </c>
@@ -20520,9 +20854,38 @@
       <c r="V13">
         <v>1</v>
       </c>
-      <c r="W13" s="1"/>
-    </row>
-    <row r="14" spans="1:31">
+      <c r="W13" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="X13" t="s">
+        <v>823</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>822</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>822</v>
+      </c>
+      <c r="AA13">
+        <v>-39</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>881</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>880</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>879</v>
+      </c>
+      <c r="AE13" s="16" t="s">
+        <v>886</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>62.295397366888402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32">
       <c r="A14" s="1" t="s">
         <v>479</v>
       </c>
@@ -20589,9 +20952,38 @@
       <c r="V14">
         <v>1</v>
       </c>
-      <c r="W14" s="1"/>
-    </row>
-    <row r="15" spans="1:31">
+      <c r="W14" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="X14" t="s">
+        <v>822</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>823</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>822</v>
+      </c>
+      <c r="AA14">
+        <v>-39</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>883</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>882</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>877</v>
+      </c>
+      <c r="AE14" s="16">
+        <v>-34</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>34.197284057404403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32">
       <c r="A15" s="1" t="s">
         <v>479</v>
       </c>
@@ -20658,9 +21050,38 @@
       <c r="V15">
         <v>1</v>
       </c>
-      <c r="W15" s="1"/>
-    </row>
-    <row r="16" spans="1:31">
+      <c r="W15" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="X15" t="s">
+        <v>824</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>823</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>824</v>
+      </c>
+      <c r="AA15">
+        <v>-39</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>883</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>882</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>878</v>
+      </c>
+      <c r="AE15" s="16" t="s">
+        <v>885</v>
+      </c>
+      <c r="AF15" s="1">
+        <v>39.377214985350797</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32">
       <c r="A16" s="1" t="s">
         <v>479</v>
       </c>
@@ -20727,9 +21148,39 @@
       <c r="V16">
         <v>1</v>
       </c>
-      <c r="W16" s="1"/>
+      <c r="W16" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="X16" t="s">
+        <v>823</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>823</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>822</v>
+      </c>
+      <c r="AA16">
+        <v>-39</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>883</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>882</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>879</v>
+      </c>
+      <c r="AE16" s="16" t="s">
+        <v>886</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>34.197284057404403</v>
+      </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{6AE5B140-7AC6-4B32-871A-93E7303764DE}"/>
@@ -20739,7 +21190,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="14">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="18">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86F1F46C-89A2-4087-9176-9DE9E8603EAE}">
           <x14:formula1>
             <xm:f>Help!$L$2:$L$5</xm:f>
@@ -20824,6 +21275,30 @@
           </x14:formula1>
           <xm:sqref>I2:I16</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50F2DA9D-BBCD-479E-8D09-550DE61A9BD9}">
+          <x14:formula1>
+            <xm:f>Help!$O$2:$O$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>W2:W16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{20F51137-79AE-44E7-9F50-256EBAF005B0}">
+          <x14:formula1>
+            <xm:f>Help!$P$2:$P$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>X2:X16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AFB1D707-7517-45EB-AD00-0D091273F1A0}">
+          <x14:formula1>
+            <xm:f>Help!$Q$2:$Q$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>Y2:Y16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A5A376C3-A2CF-4761-B652-1492A607B1C9}">
+          <x14:formula1>
+            <xm:f>Help!$R$2:$R$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>Z2:Z16</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -21991,8 +22466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332839ED-56B9-4FA1-9A11-3B9815BDFF4B}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="13.5"/>
@@ -22125,6 +22600,9 @@
       <c r="Q2" t="s">
         <v>822</v>
       </c>
+      <c r="R2" t="s">
+        <v>822</v>
+      </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
@@ -22178,6 +22656,9 @@
       <c r="Q3" t="s">
         <v>823</v>
       </c>
+      <c r="R3" t="s">
+        <v>823</v>
+      </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
@@ -22228,6 +22709,9 @@
       <c r="Q4" t="s">
         <v>824</v>
       </c>
+      <c r="R4" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="5" spans="1:18">
       <c r="B5" t="s">
@@ -22397,28 +22881,28 @@
     </row>
     <row r="29" spans="6:11">
       <c r="F29" t="s">
+        <v>871</v>
+      </c>
+      <c r="G29" t="s">
         <v>872</v>
-      </c>
-      <c r="G29" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="30" spans="6:11">
       <c r="F30">
-        <v>-38</v>
+        <v>45</v>
       </c>
       <c r="G30">
         <f>(F30-32)*5/9</f>
-        <v>-38.888888888888886</v>
+        <v>7.2222222222222223</v>
       </c>
     </row>
     <row r="31" spans="6:11">
       <c r="F31">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="G31">
         <f>(F31-32)*5/9</f>
-        <v>36.111111111111114</v>
+        <v>23.888888888888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>